<commit_message>
Adicionando modificações de Cadastro de usuários.
</commit_message>
<xml_diff>
--- a/war/excel/ImportarUsuarios.xlsx
+++ b/war/excel/ImportarUsuarios.xlsx
@@ -7,19 +7,25 @@
     <workbookView xWindow="120" yWindow="60" windowWidth="23820" windowHeight="10110"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuários" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Aluno" sheetId="4" r:id="rId1"/>
+    <sheet name="Coordenador" sheetId="1" r:id="rId2"/>
+    <sheet name="Pais" sheetId="5" r:id="rId3"/>
+    <sheet name="Professor" sheetId="6" r:id="rId4"/>
+    <sheet name="Auxiliar" sheetId="2" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="estados">Auxiliar!$C$2:$C$28</definedName>
+    <definedName name="responsavelAcademico">Auxiliar!$E$2:$E$3</definedName>
+    <definedName name="responsavelFinanceiro">Auxiliar!$F$2:$F$3</definedName>
+    <definedName name="sexo">Auxiliar!$B$2:$B$3</definedName>
+    <definedName name="situacaopais">Auxiliar!$D$2:$D$4</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
-  <si>
-    <t>Tipo Usuário</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>Primeiro Nome</t>
   </si>
@@ -39,18 +45,6 @@
     <t>CPF</t>
   </si>
   <si>
-    <t>Telefone Celular</t>
-  </si>
-  <si>
-    <t>Telefone Residencial</t>
-  </si>
-  <si>
-    <t>Telefone Comercial</t>
-  </si>
-  <si>
-    <t>Administrador</t>
-  </si>
-  <si>
     <t>Aluno</t>
   </si>
   <si>
@@ -63,17 +57,275 @@
     <t>Professor</t>
   </si>
   <si>
-    <t>Visitante</t>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Num Residencial</t>
+  </si>
+  <si>
+    <t>Bairro</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Cep</t>
+  </si>
+  <si>
+    <t>Tel Celular</t>
+  </si>
+  <si>
+    <t>Tel Residêncial</t>
+  </si>
+  <si>
+    <t>Tel Comercial</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>Situação dos Pais</t>
+  </si>
+  <si>
+    <t>Situação dos Pais(Outros)</t>
+  </si>
+  <si>
+    <t>Tipo Pais</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Resp Financeiro</t>
+  </si>
+  <si>
+    <t>Resp Acadêmico</t>
+  </si>
+  <si>
+    <t>Feminino</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Acre</t>
+  </si>
+  <si>
+    <t>Alagoas</t>
+  </si>
+  <si>
+    <t>Amapá</t>
+  </si>
+  <si>
+    <t>Amazonas</t>
+  </si>
+  <si>
+    <t>Bahia</t>
+  </si>
+  <si>
+    <t>Ceará</t>
+  </si>
+  <si>
+    <t>Distrito Federal</t>
+  </si>
+  <si>
+    <t>Espírito Santo</t>
+  </si>
+  <si>
+    <t>Goiás</t>
+  </si>
+  <si>
+    <t>Maranhão</t>
+  </si>
+  <si>
+    <t>Mato Grosso</t>
+  </si>
+  <si>
+    <t>Mato Grosso do Sul</t>
+  </si>
+  <si>
+    <t>Minas Gerais</t>
+  </si>
+  <si>
+    <t>Pará</t>
+  </si>
+  <si>
+    <t>Paraíba</t>
+  </si>
+  <si>
+    <t>Paraná</t>
+  </si>
+  <si>
+    <t>Pernambuco</t>
+  </si>
+  <si>
+    <t>Piauí</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Rio Grande do Norte</t>
+  </si>
+  <si>
+    <t>Rio Grande do Sul</t>
+  </si>
+  <si>
+    <t>Rondônia</t>
+  </si>
+  <si>
+    <t>Roraima</t>
+  </si>
+  <si>
+    <t>Santa Catarina</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>Sergipe</t>
+  </si>
+  <si>
+    <t>Tocantins</t>
+  </si>
+  <si>
+    <t>Casados</t>
+  </si>
+  <si>
+    <t>Separados</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Responsável Acadêmico</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Responsável Financeiro</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Matricula</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Formato : 25/12/2010)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Nascimento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Formato : 25/12/2010)</t>
+    </r>
+  </si>
+  <si>
+    <t>Registro Matricula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,18 +340,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -107,29 +359,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,95 +667,132 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="49.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="14" width="22.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22">
+      <c r="A1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="O3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="O4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="O5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="O6" t="s">
-        <v>15</v>
+      <c r="T1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="H2" s="1"/>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate>
     <dataRefs count="1">
-      <dataRef ref="A1:A6" sheet="Sheet2"/>
+      <dataRef ref="A1:A6" sheet="Auxiliar"/>
     </dataRefs>
   </dataConsolidate>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A32">
-      <formula1>$O$1:$O$6</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+      <formula1>sexo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
+      <formula1>estados</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2">
+      <formula1>situacaopais</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -522,60 +801,595 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="12" width="22.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="H1" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="I1" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="J1" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="K1" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="L1" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A1:A6" sheet="Auxiliar"/>
+    </dataRefs>
+  </dataConsolidate>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>sexo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
+      <formula1>estados</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="12" max="13" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A1:A6" sheet="Auxiliar"/>
+    </dataRefs>
+  </dataConsolidate>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>sexo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
+      <formula1>estados</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="12" width="22.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A1:A6" sheet="Auxiliar"/>
+    </dataRefs>
+  </dataConsolidate>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>sexo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
+      <formula1>estados</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="3:4">
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="3:4">
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="3:4">
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="3:4">
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="3:4">
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="3:4">
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="3:4">
+      <c r="D29" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>